<commit_message>
Count number of occurrences (or frequency) in a sorted array
</commit_message>
<xml_diff>
--- a/ProblemList.xlsx
+++ b/ProblemList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I511715/Desktop/codep/Arrays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5400A8-A87B-BC4E-8D90-FED6B2B7EFAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FE87D7-AD1B-0043-B891-ABDBD8284097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34480" yWindow="6360" windowWidth="28040" windowHeight="17420" xr2:uid="{81A00D1C-D504-B64A-BDD3-A19C80865734}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Problem</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>KthLargestNumber</t>
+  </si>
+  <si>
+    <t>Count number of occurrences (or frequency) in a sorted array</t>
+  </si>
+  <si>
+    <t>CountNumberOfOccurrences</t>
   </si>
 </sst>
 </file>
@@ -440,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB80EE9-32C7-C048-8D30-365F84C2A279}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,6 +514,14 @@
         <v>11</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Sort an array of 0s, 1s and 2s | Dutch National Flag problems.
</commit_message>
<xml_diff>
--- a/ProblemList.xlsx
+++ b/ProblemList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I511715/Desktop/codep/Arrays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FE87D7-AD1B-0043-B891-ABDBD8284097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95080968-15D2-D144-9D4E-A5C7A087B998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34480" yWindow="6360" windowWidth="28040" windowHeight="17420" xr2:uid="{81A00D1C-D504-B64A-BDD3-A19C80865734}"/>
+    <workbookView xWindow="42760" yWindow="9680" windowWidth="28040" windowHeight="17420" xr2:uid="{81A00D1C-D504-B64A-BDD3-A19C80865734}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Problem</t>
   </si>
@@ -78,6 +78,12 @@
   </si>
   <si>
     <t>CountNumberOfOccurrences</t>
+  </si>
+  <si>
+    <t>Sort an array of 0s, 1s and 2s</t>
+  </si>
+  <si>
+    <t>DutchNationalFlag</t>
   </si>
 </sst>
 </file>
@@ -446,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB80EE9-32C7-C048-8D30-365F84C2A279}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -522,6 +528,14 @@
         <v>13</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Sub Array With Given Sum
</commit_message>
<xml_diff>
--- a/ProblemList.xlsx
+++ b/ProblemList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I511715/Desktop/codep/Arrays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95080968-15D2-D144-9D4E-A5C7A087B998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE98AEA-71AD-034F-9769-8016C5AB8464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42760" yWindow="9680" windowWidth="28040" windowHeight="17420" xr2:uid="{81A00D1C-D504-B64A-BDD3-A19C80865734}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Problem</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>DutchNationalFlag</t>
+  </si>
+  <si>
+    <t>SubArrayWithGivenSum</t>
+  </si>
+  <si>
+    <t>Sub Array With Given Sum</t>
   </si>
 </sst>
 </file>
@@ -452,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB80EE9-32C7-C048-8D30-365F84C2A279}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -536,6 +542,14 @@
         <v>15</v>
       </c>
     </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Union and Intersection of two sorted arrays
</commit_message>
<xml_diff>
--- a/ProblemList.xlsx
+++ b/ProblemList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I511715/Desktop/codep/Arrays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90B2BF1-E5DF-804D-A24A-2CF4F8CE199A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C278AC5C-5504-754C-A7C9-C74328A95B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42760" yWindow="9680" windowWidth="28040" windowHeight="17420" xr2:uid="{81A00D1C-D504-B64A-BDD3-A19C80865734}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Problem</t>
   </si>
@@ -96,6 +96,12 @@
   </si>
   <si>
     <t>Move Negative Numbers</t>
+  </si>
+  <si>
+    <t>UnionOfTwoSortedArray</t>
+  </si>
+  <si>
+    <t>Union and Intersection of two sorted arrays</t>
   </si>
 </sst>
 </file>
@@ -464,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB80EE9-32C7-C048-8D30-365F84C2A279}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -564,6 +570,14 @@
         <v>18</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Count pairs with given sum
</commit_message>
<xml_diff>
--- a/ProblemList.xlsx
+++ b/ProblemList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I511715/Desktop/codep/Arrays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F8A623-2F9F-354C-8596-4B62FDE108BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6A3630-EDA8-9744-8B32-A2291E83AC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42760" yWindow="9680" windowWidth="28040" windowHeight="17420" xr2:uid="{81A00D1C-D504-B64A-BDD3-A19C80865734}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>Problem</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>Find the Missing Number</t>
+  </si>
+  <si>
+    <t>CountPairsWithGivenSum</t>
+  </si>
+  <si>
+    <t>Count pairs with given sum</t>
   </si>
 </sst>
 </file>
@@ -482,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB80EE9-32C7-C048-8D30-365F84C2A279}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -606,6 +612,14 @@
         <v>24</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Find duplicates in O(n) time and O(1) extra space
</commit_message>
<xml_diff>
--- a/ProblemList.xlsx
+++ b/ProblemList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I511715/Desktop/codep/Arrays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6A3630-EDA8-9744-8B32-A2291E83AC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C333A05-E19C-E140-9906-551EE6A2EF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42760" yWindow="9680" windowWidth="28040" windowHeight="17420" xr2:uid="{81A00D1C-D504-B64A-BDD3-A19C80865734}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Problem</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Count pairs with given sum</t>
+  </si>
+  <si>
+    <t>Find duplicates in O(n) time and O(1) extra space</t>
+  </si>
+  <si>
+    <t>FindDuplicate</t>
   </si>
 </sst>
 </file>
@@ -488,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB80EE9-32C7-C048-8D30-365F84C2A279}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -620,6 +626,14 @@
         <v>26</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Find common elements in three sorted arrays
</commit_message>
<xml_diff>
--- a/ProblemList.xlsx
+++ b/ProblemList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I511715/Desktop/codep/Arrays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C333A05-E19C-E140-9906-551EE6A2EF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F7981E-6260-1D4F-BAF2-AA887C335F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42760" yWindow="9680" windowWidth="28040" windowHeight="17420" xr2:uid="{81A00D1C-D504-B64A-BDD3-A19C80865734}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Problem</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>FindDuplicate</t>
+  </si>
+  <si>
+    <t>FindCommonElementsAmongThreeSortedArray</t>
+  </si>
+  <si>
+    <t>Find common elements in three sorted arrays</t>
   </si>
 </sst>
 </file>
@@ -494,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB80EE9-32C7-C048-8D30-365F84C2A279}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -634,6 +640,14 @@
         <v>29</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Find the first repeating element in an array of integers
</commit_message>
<xml_diff>
--- a/ProblemList.xlsx
+++ b/ProblemList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I511715/Desktop/codep/Arrays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F7981E-6260-1D4F-BAF2-AA887C335F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC8A38D-0B3A-C541-A0EC-864B9BAF6825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42760" yWindow="9680" windowWidth="28040" windowHeight="17420" xr2:uid="{81A00D1C-D504-B64A-BDD3-A19C80865734}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{81A00D1C-D504-B64A-BDD3-A19C80865734}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Problem</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>Find common elements in three sorted arrays</t>
+  </si>
+  <si>
+    <t>Find the first repeating element in an array of integers</t>
+  </si>
+  <si>
+    <t>FirstRepeatingElement</t>
   </si>
 </sst>
 </file>
@@ -500,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB80EE9-32C7-C048-8D30-365F84C2A279}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -648,6 +654,14 @@
         <v>30</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Find first non-repeating element in a given Array of integers
</commit_message>
<xml_diff>
--- a/ProblemList.xlsx
+++ b/ProblemList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I511715/Desktop/codep/Arrays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC8A38D-0B3A-C541-A0EC-864B9BAF6825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8849C669-90E7-1E44-939C-77940240D39D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{81A00D1C-D504-B64A-BDD3-A19C80865734}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Problem</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>FirstRepeatingElement</t>
+  </si>
+  <si>
+    <t>Find first non-repeating element in a given Array of integers</t>
+  </si>
+  <si>
+    <t>FirstNonRepeatingElement</t>
   </si>
 </sst>
 </file>
@@ -506,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB80EE9-32C7-C048-8D30-365F84C2A279}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -662,6 +668,14 @@
         <v>33</v>
       </c>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Subarrays with equal 1s and 0s
</commit_message>
<xml_diff>
--- a/ProblemList.xlsx
+++ b/ProblemList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I511715/Desktop/codep/Arrays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8849C669-90E7-1E44-939C-77940240D39D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB480C1-D42B-AD49-A67C-8B7B95507AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{81A00D1C-D504-B64A-BDD3-A19C80865734}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Problem</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>FirstNonRepeatingElement</t>
+  </si>
+  <si>
+    <t>SubArraysWithEqual1sAnd0s</t>
+  </si>
+  <si>
+    <t>Subarrays with equal 1s and 0s</t>
   </si>
 </sst>
 </file>
@@ -512,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB80EE9-32C7-C048-8D30-365F84C2A279}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -676,6 +682,14 @@
         <v>35</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rearrange array in alternating positive & negative items with O(1) extra space
</commit_message>
<xml_diff>
--- a/ProblemList.xlsx
+++ b/ProblemList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I511715/Desktop/codep/Arrays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB480C1-D42B-AD49-A67C-8B7B95507AC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F917457-0C36-DF4E-ACD2-41F166738CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17520" xr2:uid="{81A00D1C-D504-B64A-BDD3-A19C80865734}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" xr2:uid="{81A00D1C-D504-B64A-BDD3-A19C80865734}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Problem</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>Subarrays with equal 1s and 0s</t>
+  </si>
+  <si>
+    <t>RearrangeAlternatingPositiveAndNegativeNumbers</t>
+  </si>
+  <si>
+    <t>Rearrange array in alternating positive &amp; negative items with O(1) extra space</t>
   </si>
 </sst>
 </file>
@@ -518,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB80EE9-32C7-C048-8D30-365F84C2A279}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -690,6 +696,14 @@
         <v>36</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Find if there is a sub array with 0 sum
</commit_message>
<xml_diff>
--- a/ProblemList.xlsx
+++ b/ProblemList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I511715/Desktop/codep/Arrays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F917457-0C36-DF4E-ACD2-41F166738CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED15934-67A6-DC48-97B3-B4954C124235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" xr2:uid="{81A00D1C-D504-B64A-BDD3-A19C80865734}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Problem</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>Rearrange array in alternating positive &amp; negative items with O(1) extra space</t>
+  </si>
+  <si>
+    <t>Find if there is a sub array with 0 sum</t>
+  </si>
+  <si>
+    <t>SubArrayWIth0Sum</t>
   </si>
 </sst>
 </file>
@@ -524,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB80EE9-32C7-C048-8D30-365F84C2A279}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -704,6 +710,14 @@
         <v>38</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Largest Sum Contiguous Subarray (Kadane’s Algorithm)
</commit_message>
<xml_diff>
--- a/ProblemList.xlsx
+++ b/ProblemList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/I511715/Desktop/codep/Arrays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED15934-67A6-DC48-97B3-B4954C124235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F59BC7-8133-7848-8DEF-C93D23274A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" xr2:uid="{81A00D1C-D504-B64A-BDD3-A19C80865734}"/>
+    <workbookView xWindow="34560" yWindow="1460" windowWidth="30240" windowHeight="17400" xr2:uid="{81A00D1C-D504-B64A-BDD3-A19C80865734}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Problem</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>SubArrayWIth0Sum</t>
+  </si>
+  <si>
+    <t>Largest Sum Contiguous Subarray (Kadane’s Algorithm)</t>
+  </si>
+  <si>
+    <t>KadaneAlgorithm</t>
   </si>
 </sst>
 </file>
@@ -530,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB80EE9-32C7-C048-8D30-365F84C2A279}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -718,6 +724,14 @@
         <v>41</v>
       </c>
     </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>